<commit_message>
Preparations for multiverse analysis
</commit_message>
<xml_diff>
--- a/Gautret_et_al.xlsx
+++ b/Gautret_et_al.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\Documents\covid19\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC61F06-ABA8-4BE7-8880-001865940CFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{197CB1D4-FC96-431D-9141-3CF48C3045AF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="64">
   <si>
     <t>Hydroxychloroquine</t>
   </si>
@@ -222,12 +216,15 @@
   </si>
   <si>
     <t>DEATH</t>
+  </si>
+  <si>
+    <t>NoFollowup</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -269,7 +266,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normálna" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -573,19 +570,19 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E70CAD66-0443-49AB-BD9D-D414E5060F4C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N41" sqref="N41:P41"/>
+      <selection pane="bottomLeft" activeCell="Q38" sqref="Q38:Q43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2601,7 +2598,7 @@
         <v>7</v>
       </c>
       <c r="Q38" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
@@ -2654,7 +2651,7 @@
         <v>7</v>
       </c>
       <c r="Q39" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
@@ -2707,7 +2704,7 @@
         <v>7</v>
       </c>
       <c r="Q40" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
@@ -2760,7 +2757,7 @@
         <v>7</v>
       </c>
       <c r="Q41" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
@@ -2813,7 +2810,7 @@
         <v>7</v>
       </c>
       <c r="Q42" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
@@ -2866,7 +2863,7 @@
         <v>7</v>
       </c>
       <c r="Q43" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>